<commit_message>
feat: Add experiment duration calculation
</commit_message>
<xml_diff>
--- a/Data&calculations.xlsx
+++ b/Data&calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7170" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7170"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline values" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="78">
   <si>
     <t>Date</t>
   </si>
@@ -242,6 +242,27 @@
   </si>
   <si>
     <t>Clicks standard error</t>
+  </si>
+  <si>
+    <t>Calculation of required pageviews for experiment @ alpha=0.05 and beta=0.20</t>
+  </si>
+  <si>
+    <t>Gross conversion, required pageviews</t>
+  </si>
+  <si>
+    <t>Retention, required pageviews</t>
+  </si>
+  <si>
+    <t>Gross conversion, required clicks per one group</t>
+  </si>
+  <si>
+    <t>Retention, required enrollments per one group</t>
+  </si>
+  <si>
+    <t>Net conversion, required clicks per one group</t>
+  </si>
+  <si>
+    <t>Net conversion, required pageviews</t>
   </si>
 </sst>
 </file>
@@ -254,7 +275,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.000000000_-;\-* #,##0.000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -401,7 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -442,7 +463,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,6 +475,10 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1653,17 +1678,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="40.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="63.3984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.06640625" style="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -1696,6 +1723,7 @@
         <v>58</v>
       </c>
       <c r="B4" s="3">
+        <f>B2/B1</f>
         <v>0.08</v>
       </c>
     </row>
@@ -1711,7 +1739,7 @@
       <c r="A6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="37">
         <v>0.53</v>
       </c>
     </row>
@@ -1722,6 +1750,69 @@
       <c r="B7" s="3">
         <v>0.10931250000000001</v>
       </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="16">
+        <v>25835</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="36">
+        <f>2*B11/B4</f>
+        <v>645875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="36">
+        <v>39087</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="6">
+        <f>2*B13*B1/B3</f>
+        <v>4737818.1818181816</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="36">
+        <v>27413</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="36">
+        <f>2*B15/B4</f>
+        <v>685325</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B17" s="36"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B18" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4085,7 +4176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>